<commit_message>
converted grading pipeline from ipynb to scripts
</commit_message>
<xml_diff>
--- a/results/BINARY/Pretomanid.xlsx
+++ b/results/BINARY/Pretomanid.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AP50"/>
+  <dimension ref="A1:AO50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -508,7 +508,7 @@
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Num_Isolates</t>
+          <t>Present_SR</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
@@ -637,11 +637,6 @@
         </is>
       </c>
       <c r="AO1" s="1" t="inlineStr">
-        <is>
-          <t>single_lineage</t>
-        </is>
-      </c>
-      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>Phenos</t>
         </is>
@@ -778,8 +773,7 @@
           <t>Uncertain</t>
         </is>
       </c>
-      <c r="AO2" t="inlineStr"/>
-      <c r="AP2" t="inlineStr">
+      <c r="AO2" t="inlineStr">
         <is>
           <t>WHO</t>
         </is>
@@ -918,11 +912,6 @@
       </c>
       <c r="AO3" t="inlineStr">
         <is>
-          <t>4.3.4.2.1</t>
-        </is>
-      </c>
-      <c r="AP3" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -1060,11 +1049,6 @@
       </c>
       <c r="AO4" t="inlineStr">
         <is>
-          <t>2.2.1</t>
-        </is>
-      </c>
-      <c r="AP4" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -1202,11 +1186,6 @@
       </c>
       <c r="AO5" t="inlineStr">
         <is>
-          <t>2.2.1</t>
-        </is>
-      </c>
-      <c r="AP5" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -1344,11 +1323,6 @@
       </c>
       <c r="AO6" t="inlineStr">
         <is>
-          <t>2.2.1</t>
-        </is>
-      </c>
-      <c r="AP6" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -1486,11 +1460,6 @@
       </c>
       <c r="AO7" t="inlineStr">
         <is>
-          <t>2.2.2</t>
-        </is>
-      </c>
-      <c r="AP7" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -1624,8 +1593,7 @@
           <t>Uncertain</t>
         </is>
       </c>
-      <c r="AO8" t="inlineStr"/>
-      <c r="AP8" t="inlineStr">
+      <c r="AO8" t="inlineStr">
         <is>
           <t>WHO</t>
         </is>
@@ -1760,8 +1728,7 @@
           <t>Uncertain</t>
         </is>
       </c>
-      <c r="AO9" t="inlineStr"/>
-      <c r="AP9" t="inlineStr">
+      <c r="AO9" t="inlineStr">
         <is>
           <t>WHO</t>
         </is>
@@ -1896,8 +1863,7 @@
           <t>Uncertain</t>
         </is>
       </c>
-      <c r="AO10" t="inlineStr"/>
-      <c r="AP10" t="inlineStr">
+      <c r="AO10" t="inlineStr">
         <is>
           <t>WHO</t>
         </is>
@@ -2032,8 +1998,7 @@
           <t>Uncertain</t>
         </is>
       </c>
-      <c r="AO11" t="inlineStr"/>
-      <c r="AP11" t="inlineStr">
+      <c r="AO11" t="inlineStr">
         <is>
           <t>WHO</t>
         </is>
@@ -2168,8 +2133,7 @@
           <t>Uncertain</t>
         </is>
       </c>
-      <c r="AO12" t="inlineStr"/>
-      <c r="AP12" t="inlineStr">
+      <c r="AO12" t="inlineStr">
         <is>
           <t>WHO</t>
         </is>
@@ -2306,11 +2270,6 @@
       </c>
       <c r="AO13" t="inlineStr">
         <is>
-          <t>4.8</t>
-        </is>
-      </c>
-      <c r="AP13" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -2444,11 +2403,6 @@
       </c>
       <c r="AO14" t="inlineStr">
         <is>
-          <t>3.1.1</t>
-        </is>
-      </c>
-      <c r="AP14" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -2582,11 +2536,6 @@
       </c>
       <c r="AO15" t="inlineStr">
         <is>
-          <t>1.1.3</t>
-        </is>
-      </c>
-      <c r="AP15" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -2720,11 +2669,6 @@
       </c>
       <c r="AO16" t="inlineStr">
         <is>
-          <t>4.1.1.1</t>
-        </is>
-      </c>
-      <c r="AP16" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -2858,11 +2802,6 @@
       </c>
       <c r="AO17" t="inlineStr">
         <is>
-          <t>4.3.2.1</t>
-        </is>
-      </c>
-      <c r="AP17" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -2996,11 +2935,6 @@
       </c>
       <c r="AO18" t="inlineStr">
         <is>
-          <t>BOV_AFRI</t>
-        </is>
-      </c>
-      <c r="AP18" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -3134,11 +3068,6 @@
       </c>
       <c r="AO19" t="inlineStr">
         <is>
-          <t>4.3.4.2.1</t>
-        </is>
-      </c>
-      <c r="AP19" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -3272,11 +3201,6 @@
       </c>
       <c r="AO20" t="inlineStr">
         <is>
-          <t>4.3.4.2.1</t>
-        </is>
-      </c>
-      <c r="AP20" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -3410,11 +3334,6 @@
       </c>
       <c r="AO21" t="inlineStr">
         <is>
-          <t>2.2.1.1</t>
-        </is>
-      </c>
-      <c r="AP21" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -3548,11 +3467,6 @@
       </c>
       <c r="AO22" t="inlineStr">
         <is>
-          <t>4.3.3</t>
-        </is>
-      </c>
-      <c r="AP22" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -3686,11 +3600,6 @@
       </c>
       <c r="AO23" t="inlineStr">
         <is>
-          <t>4.3.2</t>
-        </is>
-      </c>
-      <c r="AP23" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -3822,8 +3731,7 @@
           <t>Uncertain</t>
         </is>
       </c>
-      <c r="AO24" t="inlineStr"/>
-      <c r="AP24" t="inlineStr">
+      <c r="AO24" t="inlineStr">
         <is>
           <t>WHO</t>
         </is>
@@ -3958,11 +3866,6 @@
       </c>
       <c r="AO25" t="inlineStr">
         <is>
-          <t>4.3.3</t>
-        </is>
-      </c>
-      <c r="AP25" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -4096,11 +3999,6 @@
       </c>
       <c r="AO26" t="inlineStr">
         <is>
-          <t>2.2.1</t>
-        </is>
-      </c>
-      <c r="AP26" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -4234,11 +4132,6 @@
       </c>
       <c r="AO27" t="inlineStr">
         <is>
-          <t>2.2.1</t>
-        </is>
-      </c>
-      <c r="AP27" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -4372,11 +4265,6 @@
       </c>
       <c r="AO28" t="inlineStr">
         <is>
-          <t>4.3.4.2.1</t>
-        </is>
-      </c>
-      <c r="AP28" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -4510,11 +4398,6 @@
       </c>
       <c r="AO29" t="inlineStr">
         <is>
-          <t>4.8</t>
-        </is>
-      </c>
-      <c r="AP29" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -4648,11 +4531,6 @@
       </c>
       <c r="AO30" t="inlineStr">
         <is>
-          <t>BOV_AFRI</t>
-        </is>
-      </c>
-      <c r="AP30" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -4786,11 +4664,6 @@
       </c>
       <c r="AO31" t="inlineStr">
         <is>
-          <t>3.1.2.1</t>
-        </is>
-      </c>
-      <c r="AP31" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -4924,11 +4797,6 @@
       </c>
       <c r="AO32" t="inlineStr">
         <is>
-          <t>4.1.1.1</t>
-        </is>
-      </c>
-      <c r="AP32" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -5062,11 +4930,6 @@
       </c>
       <c r="AO33" t="inlineStr">
         <is>
-          <t>4.6.2</t>
-        </is>
-      </c>
-      <c r="AP33" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -5200,11 +5063,6 @@
       </c>
       <c r="AO34" t="inlineStr">
         <is>
-          <t>4.9</t>
-        </is>
-      </c>
-      <c r="AP34" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -5338,11 +5196,6 @@
       </c>
       <c r="AO35" t="inlineStr">
         <is>
-          <t>2.2.1</t>
-        </is>
-      </c>
-      <c r="AP35" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -5476,11 +5329,6 @@
       </c>
       <c r="AO36" t="inlineStr">
         <is>
-          <t>1.2.2</t>
-        </is>
-      </c>
-      <c r="AP36" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -5614,11 +5462,6 @@
       </c>
       <c r="AO37" t="inlineStr">
         <is>
-          <t>2.2.1</t>
-        </is>
-      </c>
-      <c r="AP37" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -5752,11 +5595,6 @@
       </c>
       <c r="AO38" t="inlineStr">
         <is>
-          <t>1.1.2</t>
-        </is>
-      </c>
-      <c r="AP38" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -5890,11 +5728,6 @@
       </c>
       <c r="AO39" t="inlineStr">
         <is>
-          <t>4.4.1.1</t>
-        </is>
-      </c>
-      <c r="AP39" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -6028,11 +5861,6 @@
       </c>
       <c r="AO40" t="inlineStr">
         <is>
-          <t>4.3.3</t>
-        </is>
-      </c>
-      <c r="AP40" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -6166,11 +5994,6 @@
       </c>
       <c r="AO41" t="inlineStr">
         <is>
-          <t>2.1</t>
-        </is>
-      </c>
-      <c r="AP41" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -6304,11 +6127,6 @@
       </c>
       <c r="AO42" t="inlineStr">
         <is>
-          <t>2.2.1</t>
-        </is>
-      </c>
-      <c r="AP42" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -6442,11 +6260,6 @@
       </c>
       <c r="AO43" t="inlineStr">
         <is>
-          <t>4.1.2</t>
-        </is>
-      </c>
-      <c r="AP43" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -6578,8 +6391,7 @@
           <t>Neutral</t>
         </is>
       </c>
-      <c r="AO44" t="inlineStr"/>
-      <c r="AP44" t="inlineStr">
+      <c r="AO44" t="inlineStr">
         <is>
           <t>WHO</t>
         </is>
@@ -6714,11 +6526,6 @@
       </c>
       <c r="AO45" t="inlineStr">
         <is>
-          <t>1.2.1</t>
-        </is>
-      </c>
-      <c r="AP45" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -6852,11 +6659,6 @@
       </c>
       <c r="AO46" t="inlineStr">
         <is>
-          <t>1.2.1</t>
-        </is>
-      </c>
-      <c r="AP46" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -6990,11 +6792,6 @@
       </c>
       <c r="AO47" t="inlineStr">
         <is>
-          <t>1.2.1</t>
-        </is>
-      </c>
-      <c r="AP47" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -7128,11 +6925,6 @@
       </c>
       <c r="AO48" t="inlineStr">
         <is>
-          <t>1.2.1</t>
-        </is>
-      </c>
-      <c r="AP48" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -7266,11 +7058,6 @@
       </c>
       <c r="AO49" t="inlineStr">
         <is>
-          <t>1.2.1</t>
-        </is>
-      </c>
-      <c r="AP49" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -7403,11 +7190,6 @@
         </is>
       </c>
       <c r="AO50" t="inlineStr">
-        <is>
-          <t>1.2.1</t>
-        </is>
-      </c>
-      <c r="AP50" t="inlineStr">
         <is>
           <t>WHO</t>
         </is>
@@ -7424,7 +7206,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AP4"/>
+  <dimension ref="A1:AO4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7505,7 +7287,7 @@
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Num_Isolates</t>
+          <t>Present_SR</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
@@ -7634,11 +7416,6 @@
         </is>
       </c>
       <c r="AO1" s="1" t="inlineStr">
-        <is>
-          <t>single_lineage</t>
-        </is>
-      </c>
-      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>Phenos</t>
         </is>
@@ -7771,8 +7548,7 @@
           <t>Assoc w R</t>
         </is>
       </c>
-      <c r="AO2" t="inlineStr"/>
-      <c r="AP2" t="inlineStr">
+      <c r="AO2" t="inlineStr">
         <is>
           <t>WHO</t>
         </is>
@@ -7905,8 +7681,7 @@
           <t>Uncertain</t>
         </is>
       </c>
-      <c r="AO3" t="inlineStr"/>
-      <c r="AP3" t="inlineStr">
+      <c r="AO3" t="inlineStr">
         <is>
           <t>WHO</t>
         </is>
@@ -8035,8 +7810,7 @@
           <t>Uncertain</t>
         </is>
       </c>
-      <c r="AO4" t="inlineStr"/>
-      <c r="AP4" t="inlineStr">
+      <c r="AO4" t="inlineStr">
         <is>
           <t>WHO</t>
         </is>
@@ -8053,7 +7827,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AP39"/>
+  <dimension ref="A1:AO39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8134,7 +7908,7 @@
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Num_Isolates</t>
+          <t>Present_SR</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
@@ -8263,11 +8037,6 @@
         </is>
       </c>
       <c r="AO1" s="1" t="inlineStr">
-        <is>
-          <t>single_lineage</t>
-        </is>
-      </c>
-      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>Phenos</t>
         </is>
@@ -8404,11 +8173,6 @@
       </c>
       <c r="AO2" t="inlineStr">
         <is>
-          <t>1.2.1</t>
-        </is>
-      </c>
-      <c r="AP2" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -8544,11 +8308,6 @@
       </c>
       <c r="AO3" t="inlineStr">
         <is>
-          <t>1.2.1</t>
-        </is>
-      </c>
-      <c r="AP3" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -8682,8 +8441,7 @@
           <t>Uncertain</t>
         </is>
       </c>
-      <c r="AO4" t="inlineStr"/>
-      <c r="AP4" t="inlineStr">
+      <c r="AO4" t="inlineStr">
         <is>
           <t>WHO</t>
         </is>
@@ -8820,11 +8578,6 @@
       </c>
       <c r="AO5" t="inlineStr">
         <is>
-          <t>4.3.4.2.1</t>
-        </is>
-      </c>
-      <c r="AP5" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -8960,11 +8713,6 @@
       </c>
       <c r="AO6" t="inlineStr">
         <is>
-          <t>4.4.1.1</t>
-        </is>
-      </c>
-      <c r="AP6" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -9100,11 +8848,6 @@
       </c>
       <c r="AO7" t="inlineStr">
         <is>
-          <t>4.4.1.1</t>
-        </is>
-      </c>
-      <c r="AP7" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -9238,8 +8981,7 @@
           <t>Uncertain</t>
         </is>
       </c>
-      <c r="AO8" t="inlineStr"/>
-      <c r="AP8" t="inlineStr">
+      <c r="AO8" t="inlineStr">
         <is>
           <t>WHO</t>
         </is>
@@ -9374,8 +9116,7 @@
           <t>Uncertain</t>
         </is>
       </c>
-      <c r="AO9" t="inlineStr"/>
-      <c r="AP9" t="inlineStr">
+      <c r="AO9" t="inlineStr">
         <is>
           <t>WHO</t>
         </is>
@@ -9510,8 +9251,7 @@
           <t>Uncertain</t>
         </is>
       </c>
-      <c r="AO10" t="inlineStr"/>
-      <c r="AP10" t="inlineStr">
+      <c r="AO10" t="inlineStr">
         <is>
           <t>WHO</t>
         </is>
@@ -9646,8 +9386,7 @@
           <t>Uncertain</t>
         </is>
       </c>
-      <c r="AO11" t="inlineStr"/>
-      <c r="AP11" t="inlineStr">
+      <c r="AO11" t="inlineStr">
         <is>
           <t>WHO</t>
         </is>
@@ -9782,8 +9521,7 @@
           <t>Uncertain</t>
         </is>
       </c>
-      <c r="AO12" t="inlineStr"/>
-      <c r="AP12" t="inlineStr">
+      <c r="AO12" t="inlineStr">
         <is>
           <t>WHO</t>
         </is>
@@ -9918,8 +9656,7 @@
           <t>Uncertain</t>
         </is>
       </c>
-      <c r="AO13" t="inlineStr"/>
-      <c r="AP13" t="inlineStr">
+      <c r="AO13" t="inlineStr">
         <is>
           <t>WHO</t>
         </is>
@@ -10054,8 +9791,7 @@
           <t>Uncertain</t>
         </is>
       </c>
-      <c r="AO14" t="inlineStr"/>
-      <c r="AP14" t="inlineStr">
+      <c r="AO14" t="inlineStr">
         <is>
           <t>WHO</t>
         </is>
@@ -10190,8 +9926,7 @@
           <t>Uncertain</t>
         </is>
       </c>
-      <c r="AO15" t="inlineStr"/>
-      <c r="AP15" t="inlineStr">
+      <c r="AO15" t="inlineStr">
         <is>
           <t>WHO</t>
         </is>
@@ -10326,8 +10061,7 @@
           <t>Uncertain</t>
         </is>
       </c>
-      <c r="AO16" t="inlineStr"/>
-      <c r="AP16" t="inlineStr">
+      <c r="AO16" t="inlineStr">
         <is>
           <t>WHO</t>
         </is>
@@ -10462,8 +10196,7 @@
           <t>Uncertain</t>
         </is>
       </c>
-      <c r="AO17" t="inlineStr"/>
-      <c r="AP17" t="inlineStr">
+      <c r="AO17" t="inlineStr">
         <is>
           <t>WHO</t>
         </is>
@@ -10598,8 +10331,7 @@
           <t>Uncertain</t>
         </is>
       </c>
-      <c r="AO18" t="inlineStr"/>
-      <c r="AP18" t="inlineStr">
+      <c r="AO18" t="inlineStr">
         <is>
           <t>WHO</t>
         </is>
@@ -10734,8 +10466,7 @@
           <t>Uncertain</t>
         </is>
       </c>
-      <c r="AO19" t="inlineStr"/>
-      <c r="AP19" t="inlineStr">
+      <c r="AO19" t="inlineStr">
         <is>
           <t>WHO</t>
         </is>
@@ -10872,11 +10603,6 @@
       </c>
       <c r="AO20" t="inlineStr">
         <is>
-          <t>4.9</t>
-        </is>
-      </c>
-      <c r="AP20" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -11010,11 +10736,6 @@
       </c>
       <c r="AO21" t="inlineStr">
         <is>
-          <t>4.1.1.1</t>
-        </is>
-      </c>
-      <c r="AP21" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -11148,11 +10869,6 @@
       </c>
       <c r="AO22" t="inlineStr">
         <is>
-          <t>4.1.1.3</t>
-        </is>
-      </c>
-      <c r="AP22" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -11286,11 +11002,6 @@
       </c>
       <c r="AO23" t="inlineStr">
         <is>
-          <t>4.1.1.3</t>
-        </is>
-      </c>
-      <c r="AP23" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -11424,11 +11135,6 @@
       </c>
       <c r="AO24" t="inlineStr">
         <is>
-          <t>BOV_AFRI</t>
-        </is>
-      </c>
-      <c r="AP24" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -11562,11 +11268,6 @@
       </c>
       <c r="AO25" t="inlineStr">
         <is>
-          <t>4.3.4.2.1</t>
-        </is>
-      </c>
-      <c r="AP25" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -11700,11 +11401,6 @@
       </c>
       <c r="AO26" t="inlineStr">
         <is>
-          <t>1.1.3</t>
-        </is>
-      </c>
-      <c r="AP26" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -11838,11 +11534,6 @@
       </c>
       <c r="AO27" t="inlineStr">
         <is>
-          <t>4.6.2.2</t>
-        </is>
-      </c>
-      <c r="AP27" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -11976,11 +11667,6 @@
       </c>
       <c r="AO28" t="inlineStr">
         <is>
-          <t>4.1.1.3</t>
-        </is>
-      </c>
-      <c r="AP28" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -12114,11 +11800,6 @@
       </c>
       <c r="AO29" t="inlineStr">
         <is>
-          <t>1.1.2</t>
-        </is>
-      </c>
-      <c r="AP29" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -12252,11 +11933,6 @@
       </c>
       <c r="AO30" t="inlineStr">
         <is>
-          <t>2.2.1</t>
-        </is>
-      </c>
-      <c r="AP30" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -12390,11 +12066,6 @@
       </c>
       <c r="AO31" t="inlineStr">
         <is>
-          <t>2.2.1</t>
-        </is>
-      </c>
-      <c r="AP31" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -12528,11 +12199,6 @@
       </c>
       <c r="AO32" t="inlineStr">
         <is>
-          <t>1.1.3</t>
-        </is>
-      </c>
-      <c r="AP32" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -12666,11 +12332,6 @@
       </c>
       <c r="AO33" t="inlineStr">
         <is>
-          <t>2.2.1</t>
-        </is>
-      </c>
-      <c r="AP33" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -12804,11 +12465,6 @@
       </c>
       <c r="AO34" t="inlineStr">
         <is>
-          <t>4.1.1</t>
-        </is>
-      </c>
-      <c r="AP34" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -12942,11 +12598,6 @@
       </c>
       <c r="AO35" t="inlineStr">
         <is>
-          <t>1.1.2</t>
-        </is>
-      </c>
-      <c r="AP35" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -13080,11 +12731,6 @@
       </c>
       <c r="AO36" t="inlineStr">
         <is>
-          <t>4.2.1</t>
-        </is>
-      </c>
-      <c r="AP36" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -13218,11 +12864,6 @@
       </c>
       <c r="AO37" t="inlineStr">
         <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="AP37" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -13356,11 +12997,6 @@
       </c>
       <c r="AO38" t="inlineStr">
         <is>
-          <t>2.2.1</t>
-        </is>
-      </c>
-      <c r="AP38" t="inlineStr">
-        <is>
           <t>WHO</t>
         </is>
       </c>
@@ -13493,11 +13129,6 @@
         </is>
       </c>
       <c r="AO39" t="inlineStr">
-        <is>
-          <t>4.3.3</t>
-        </is>
-      </c>
-      <c r="AP39" t="inlineStr">
         <is>
           <t>WHO</t>
         </is>

</xml_diff>